<commit_message>
findings in test-suite Fixes #397
</commit_message>
<xml_diff>
--- a/testing/RegistryOffice+testcase.docs.xlsx
+++ b/testing/RegistryOffice+testcase.docs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IS00759329\Desktop\Telefonica\ApplicationPattern\ApplicationPattern_v2\testSuites_docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F61C76AF-80A6-4393-A56F-9DCD7E773315}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1FFC824-674A-4AFD-8D38-9B12BD828181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5C9BFFBC-C797-4681-8DC0-981A45E67C76}"/>
+    <workbookView xWindow="285" yWindow="270" windowWidth="20205" windowHeight="10650" xr2:uid="{5C9BFFBC-C797-4681-8DC0-981A45E67C76}"/>
   </bookViews>
   <sheets>
     <sheet name="ServiceLayer" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1182" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1183" uniqueCount="294">
   <si>
     <t>Registry Office</t>
   </si>
@@ -1537,6 +1537,14 @@
   - all attributes filled with random dummy values (that comply specification)
    - reasonable parameter
    - operation-key from above</t>
+  </si>
+  <si>
+    <t>#### Clearing:
+- PUT initial newRelease/application-name
+- PUT initial newRelease/release-number
+- PUT initial newRelease/protocol
+- PUT initial newRelease/address
+- PUT initial newRelease/port</t>
   </si>
 </sst>
 </file>
@@ -1982,20 +1990,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2316,10 +2324,10 @@
   <dimension ref="A1:O206"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="F26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B129" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="H31" sqref="H31"/>
+      <selection pane="bottomRight" activeCell="C132" sqref="C132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2413,7 +2421,7 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="68" t="s">
+      <c r="A4" s="70" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="17" t="s">
@@ -2469,7 +2477,7 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="240" x14ac:dyDescent="0.25">
-      <c r="A5" s="68"/>
+      <c r="A5" s="70"/>
       <c r="B5" s="18" t="s">
         <v>43</v>
       </c>
@@ -2619,7 +2627,7 @@
       </c>
     </row>
     <row r="6" spans="1:14" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="68"/>
+      <c r="A6" s="70"/>
       <c r="B6" s="18" t="s">
         <v>44</v>
       </c>
@@ -2691,7 +2699,7 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="68"/>
+      <c r="A7" s="70"/>
       <c r="B7" s="19" t="s">
         <v>45</v>
       </c>
@@ -2755,7 +2763,7 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="68" t="s">
+      <c r="A8" s="70" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="20" t="s">
@@ -2811,7 +2819,7 @@
       </c>
     </row>
     <row r="9" spans="1:14" ht="255.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="68"/>
+      <c r="A9" s="70"/>
       <c r="B9" s="21" t="s">
         <v>47</v>
       </c>
@@ -2967,7 +2975,7 @@
       </c>
     </row>
     <row r="10" spans="1:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="68"/>
+      <c r="A10" s="70"/>
       <c r="B10" s="21" t="s">
         <v>48</v>
       </c>
@@ -3033,7 +3041,7 @@
       </c>
     </row>
     <row r="11" spans="1:14" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="68"/>
+      <c r="A11" s="70"/>
       <c r="B11" s="19" t="str">
         <f t="shared" ref="B11" si="9">$B7</f>
         <v>#### Clearing:
@@ -3103,7 +3111,7 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="68" t="s">
+      <c r="A12" s="70" t="s">
         <v>5</v>
       </c>
       <c r="B12" s="20" t="s">
@@ -3159,7 +3167,7 @@
       </c>
     </row>
     <row r="13" spans="1:14" ht="270" x14ac:dyDescent="0.25">
-      <c r="A13" s="70"/>
+      <c r="A13" s="72"/>
       <c r="B13" s="21" t="s">
         <v>50</v>
       </c>
@@ -3315,7 +3323,7 @@
       </c>
     </row>
     <row r="14" spans="1:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="70"/>
+      <c r="A14" s="72"/>
       <c r="B14" s="21" t="s">
         <v>51</v>
       </c>
@@ -3381,7 +3389,7 @@
       </c>
     </row>
     <row r="15" spans="1:14" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="70"/>
+      <c r="A15" s="72"/>
       <c r="B15" s="19" t="str">
         <f t="shared" ref="B15" si="14">$B7</f>
         <v>#### Clearing:
@@ -3451,7 +3459,7 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="68" t="s">
+      <c r="A16" s="70" t="s">
         <v>6</v>
       </c>
       <c r="B16" s="20" t="s">
@@ -3507,7 +3515,7 @@
       </c>
     </row>
     <row r="17" spans="1:14" ht="270" x14ac:dyDescent="0.25">
-      <c r="A17" s="68"/>
+      <c r="A17" s="70"/>
       <c r="B17" s="21" t="s">
         <v>53</v>
       </c>
@@ -3663,7 +3671,7 @@
       </c>
     </row>
     <row r="18" spans="1:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="68"/>
+      <c r="A18" s="70"/>
       <c r="B18" s="21" t="s">
         <v>51</v>
       </c>
@@ -3729,7 +3737,7 @@
       </c>
     </row>
     <row r="19" spans="1:14" ht="60" x14ac:dyDescent="0.25">
-      <c r="A19" s="68"/>
+      <c r="A19" s="70"/>
       <c r="B19" s="19" t="str">
         <f t="shared" ref="B19" si="19">$B7</f>
         <v>#### Clearing:
@@ -3799,7 +3807,7 @@
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="68" t="s">
+      <c r="A20" s="70" t="s">
         <v>7</v>
       </c>
       <c r="B20" s="20" t="s">
@@ -3855,7 +3863,7 @@
       </c>
     </row>
     <row r="21" spans="1:14" ht="270" x14ac:dyDescent="0.25">
-      <c r="A21" s="68"/>
+      <c r="A21" s="70"/>
       <c r="B21" s="21" t="s">
         <v>55</v>
       </c>
@@ -4011,7 +4019,7 @@
       </c>
     </row>
     <row r="22" spans="1:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="68"/>
+      <c r="A22" s="70"/>
       <c r="B22" s="21" t="s">
         <v>51</v>
       </c>
@@ -4077,7 +4085,7 @@
       </c>
     </row>
     <row r="23" spans="1:14" ht="60" x14ac:dyDescent="0.25">
-      <c r="A23" s="68"/>
+      <c r="A23" s="70"/>
       <c r="B23" s="19" t="str">
         <f t="shared" ref="B23" si="24">$B7</f>
         <v>#### Clearing:
@@ -4147,7 +4155,7 @@
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="68" t="s">
+      <c r="A24" s="70" t="s">
         <v>8</v>
       </c>
       <c r="B24" s="20" t="s">
@@ -4203,7 +4211,7 @@
       </c>
     </row>
     <row r="25" spans="1:14" ht="255" x14ac:dyDescent="0.25">
-      <c r="A25" s="68"/>
+      <c r="A25" s="70"/>
       <c r="B25" s="21" t="s">
         <v>57</v>
       </c>
@@ -4252,7 +4260,7 @@
 - BUT operationKey parameter missing (does not mean empty string)</v>
       </c>
       <c r="G25" s="58" t="str">
-        <f t="shared" ref="G25:H25" si="26">SUBSTITUTE(G$5,"  -operation-key from above", "")&amp;"
+        <f t="shared" ref="G25" si="26">SUBSTITUTE(G$5,"  -operation-key from above", "")&amp;"
 - BUT operationKey parameter missing (does not mean empty string)"</f>
         <v>#### Preparation:
 - GETing CC (/core-model-1-4:control-construct)
@@ -4335,7 +4343,7 @@
       </c>
     </row>
     <row r="26" spans="1:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="68"/>
+      <c r="A26" s="70"/>
       <c r="B26" s="21" t="s">
         <v>58</v>
       </c>
@@ -4397,7 +4405,7 @@
       </c>
     </row>
     <row r="27" spans="1:14" ht="60" x14ac:dyDescent="0.25">
-      <c r="A27" s="68"/>
+      <c r="A27" s="70"/>
       <c r="B27" s="19" t="str">
         <f t="shared" ref="B27" si="29">$B7</f>
         <v>#### Clearing:
@@ -4463,7 +4471,7 @@
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" s="68" t="s">
+      <c r="A28" s="70" t="s">
         <v>9</v>
       </c>
       <c r="B28" s="20" t="s">
@@ -4519,7 +4527,7 @@
       </c>
     </row>
     <row r="29" spans="1:14" ht="255" x14ac:dyDescent="0.25">
-      <c r="A29" s="68"/>
+      <c r="A29" s="70"/>
       <c r="B29" s="21" t="s">
         <v>60</v>
       </c>
@@ -4568,7 +4576,7 @@
   - BUT operationKey with random DummyValue</v>
       </c>
       <c r="G29" s="58" t="str">
-        <f t="shared" ref="G29:H29" si="31">SUBSTITUTE(G$5,"  -operation-key from above", "")&amp;"
+        <f t="shared" ref="G29" si="31">SUBSTITUTE(G$5,"  -operation-key from above", "")&amp;"
   - BUT operationKey with random DummyValue"</f>
         <v>#### Preparation:
 - GETing CC (/core-model-1-4:control-construct)
@@ -4651,7 +4659,7 @@
       </c>
     </row>
     <row r="30" spans="1:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="68"/>
+      <c r="A30" s="70"/>
       <c r="B30" s="21" t="s">
         <v>58</v>
       </c>
@@ -4713,7 +4721,7 @@
       </c>
     </row>
     <row r="31" spans="1:14" ht="60" x14ac:dyDescent="0.25">
-      <c r="A31" s="68"/>
+      <c r="A31" s="70"/>
       <c r="B31" s="19" t="str">
         <f t="shared" ref="B31" si="34">$B7</f>
         <v>#### Clearing:
@@ -4779,7 +4787,7 @@
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" s="68" t="s">
+      <c r="A32" s="70" t="s">
         <v>10</v>
       </c>
       <c r="B32" s="20" t="s">
@@ -4835,7 +4843,7 @@
       </c>
     </row>
     <row r="33" spans="1:14" ht="240" x14ac:dyDescent="0.25">
-      <c r="A33" s="68"/>
+      <c r="A33" s="70"/>
       <c r="B33" s="21" t="s">
         <v>62</v>
       </c>
@@ -4972,7 +4980,7 @@
       </c>
     </row>
     <row r="34" spans="1:14" ht="75" x14ac:dyDescent="0.25">
-      <c r="A34" s="68"/>
+      <c r="A34" s="70"/>
       <c r="B34" s="21" t="s">
         <v>63</v>
       </c>
@@ -5050,7 +5058,7 @@
       </c>
     </row>
     <row r="35" spans="1:14" ht="60" x14ac:dyDescent="0.25">
-      <c r="A35" s="68"/>
+      <c r="A35" s="70"/>
       <c r="B35" s="19" t="str">
         <f t="shared" ref="B35" si="40">$B7</f>
         <v>#### Clearing:
@@ -5120,7 +5128,7 @@
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A36" s="68" t="s">
+      <c r="A36" s="70" t="s">
         <v>11</v>
       </c>
       <c r="B36" s="20" t="s">
@@ -5176,7 +5184,7 @@
       </c>
     </row>
     <row r="37" spans="1:14" ht="240" x14ac:dyDescent="0.25">
-      <c r="A37" s="68"/>
+      <c r="A37" s="70"/>
       <c r="B37" s="21" t="s">
         <v>62</v>
       </c>
@@ -5312,8 +5320,8 @@
    - reasonable parameter</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="45" x14ac:dyDescent="0.25">
-      <c r="A38" s="68"/>
+    <row r="38" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+      <c r="A38" s="70"/>
       <c r="B38" s="21" t="s">
         <v>65</v>
       </c>
@@ -5391,7 +5399,7 @@
       </c>
     </row>
     <row r="39" spans="1:14" ht="60" x14ac:dyDescent="0.25">
-      <c r="A39" s="68"/>
+      <c r="A39" s="70"/>
       <c r="B39" s="19" t="str">
         <f t="shared" ref="B39" si="46">$B7</f>
         <v>#### Clearing:
@@ -5461,7 +5469,7 @@
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A40" s="68" t="s">
+      <c r="A40" s="70" t="s">
         <v>12</v>
       </c>
       <c r="B40" s="20" t="s">
@@ -5812,7 +5820,7 @@
       </c>
     </row>
     <row r="44" spans="1:14" ht="45" x14ac:dyDescent="0.25">
-      <c r="A44" s="68" t="s">
+      <c r="A44" s="70" t="s">
         <v>13</v>
       </c>
       <c r="B44" s="20" t="s">
@@ -6392,7 +6400,7 @@
       <c r="N49" s="42"/>
     </row>
     <row r="50" spans="1:14" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="68" t="s">
+      <c r="A50" s="70" t="s">
         <v>15</v>
       </c>
       <c r="B50" s="24" t="s">
@@ -6576,7 +6584,7 @@
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A54" s="71" t="s">
+      <c r="A54" s="68" t="s">
         <v>16</v>
       </c>
       <c r="B54" s="24" t="s">
@@ -6620,7 +6628,7 @@
       </c>
     </row>
     <row r="55" spans="1:14" ht="195" x14ac:dyDescent="0.25">
-      <c r="A55" s="71"/>
+      <c r="A55" s="68"/>
       <c r="B55" s="25" t="s">
         <v>77</v>
       </c>
@@ -6694,7 +6702,7 @@
       </c>
     </row>
     <row r="56" spans="1:14" ht="75" x14ac:dyDescent="0.25">
-      <c r="A56" s="71"/>
+      <c r="A56" s="68"/>
       <c r="B56" s="26" t="s">
         <v>78</v>
       </c>
@@ -6736,7 +6744,7 @@
       </c>
     </row>
     <row r="57" spans="1:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="A57" s="71"/>
+      <c r="A57" s="68"/>
       <c r="B57" s="27" t="s">
         <v>75</v>
       </c>
@@ -6820,7 +6828,7 @@
       </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A59" s="68" t="s">
+      <c r="A59" s="70" t="s">
         <v>17</v>
       </c>
       <c r="B59" s="20" t="s">
@@ -7124,7 +7132,7 @@
       </c>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A63" s="68" t="s">
+      <c r="A63" s="70" t="s">
         <v>18</v>
       </c>
       <c r="B63" s="20" t="s">
@@ -7168,7 +7176,7 @@
       </c>
     </row>
     <row r="64" spans="1:14" ht="270" x14ac:dyDescent="0.25">
-      <c r="A64" s="68"/>
+      <c r="A64" s="70"/>
       <c r="B64" s="21" t="s">
         <v>85</v>
       </c>
@@ -7323,7 +7331,7 @@
       </c>
     </row>
     <row r="65" spans="1:14" ht="45" x14ac:dyDescent="0.25">
-      <c r="A65" s="68"/>
+      <c r="A65" s="70"/>
       <c r="B65" s="21" t="s">
         <v>86</v>
       </c>
@@ -7385,7 +7393,7 @@
       </c>
     </row>
     <row r="66" spans="1:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="A66" s="68"/>
+      <c r="A66" s="70"/>
       <c r="B66" s="28" t="s">
         <v>75</v>
       </c>
@@ -7447,7 +7455,7 @@
       </c>
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A67" s="68" t="s">
+      <c r="A67" s="70" t="s">
         <v>19</v>
       </c>
       <c r="B67" s="20" t="s">
@@ -7503,7 +7511,7 @@
       </c>
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A68" s="68"/>
+      <c r="A68" s="70"/>
       <c r="B68" s="21"/>
       <c r="C68" s="48" t="s">
         <v>113</v>
@@ -8984,7 +8992,7 @@
       <c r="N99" s="67"/>
     </row>
     <row r="100" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A100" s="68" t="s">
+      <c r="A100" s="70" t="s">
         <v>20</v>
       </c>
       <c r="B100" s="20" t="s">
@@ -9040,7 +9048,7 @@
       </c>
     </row>
     <row r="101" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A101" s="68"/>
+      <c r="A101" s="70"/>
       <c r="B101" s="21"/>
       <c r="C101" s="48" t="s">
         <v>163</v>
@@ -10079,7 +10087,7 @@
       <c r="N125" s="67"/>
     </row>
     <row r="126" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A126" s="68" t="s">
+      <c r="A126" s="70" t="s">
         <v>21</v>
       </c>
       <c r="B126" s="20" t="s">
@@ -10123,7 +10131,7 @@
       </c>
     </row>
     <row r="127" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A127" s="68"/>
+      <c r="A127" s="70"/>
       <c r="B127" s="25"/>
       <c r="C127" s="50" t="s">
         <v>122</v>
@@ -10401,17 +10409,15 @@
         <v>224</v>
       </c>
     </row>
-    <row r="131" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:14" ht="90" x14ac:dyDescent="0.25">
       <c r="A131" s="69"/>
       <c r="B131" s="18" t="str">
         <f>$B7</f>
         <v>#### Clearing:
 - not applicable</v>
       </c>
-      <c r="C131" s="52" t="str">
-        <f>$B7</f>
-        <v>#### Clearing:
-- not applicable</v>
+      <c r="C131" s="52" t="s">
+        <v>293</v>
       </c>
       <c r="D131" s="52" t="str">
         <f>$B7</f>
@@ -10577,7 +10583,7 @@
       <c r="N136" s="66"/>
     </row>
     <row r="137" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A137" s="68" t="s">
+      <c r="A137" s="70" t="s">
         <v>22</v>
       </c>
       <c r="B137" s="24" t="s">
@@ -10621,7 +10627,7 @@
       </c>
     </row>
     <row r="138" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A138" s="68"/>
+      <c r="A138" s="70"/>
       <c r="B138" s="26"/>
       <c r="C138" s="53"/>
       <c r="D138" s="67" t="s">
@@ -10659,7 +10665,7 @@
       </c>
     </row>
     <row r="139" spans="1:14" ht="180" x14ac:dyDescent="0.25">
-      <c r="A139" s="68"/>
+      <c r="A139" s="70"/>
       <c r="B139" s="25" t="s">
         <v>97</v>
       </c>
@@ -10701,7 +10707,7 @@
       </c>
     </row>
     <row r="140" spans="1:14" ht="149.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="68"/>
+      <c r="A140" s="70"/>
       <c r="B140" s="26" t="s">
         <v>98</v>
       </c>
@@ -10743,7 +10749,7 @@
       </c>
     </row>
     <row r="141" spans="1:14" ht="90" x14ac:dyDescent="0.25">
-      <c r="A141" s="68"/>
+      <c r="A141" s="70"/>
       <c r="B141" s="26" t="s">
         <v>75</v>
       </c>
@@ -10915,7 +10921,7 @@
       <c r="N147" s="67"/>
     </row>
     <row r="148" spans="1:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="A148" s="68" t="s">
+      <c r="A148" s="70" t="s">
         <v>23</v>
       </c>
       <c r="B148" s="20" t="s">
@@ -10959,7 +10965,7 @@
       </c>
     </row>
     <row r="149" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A149" s="68"/>
+      <c r="A149" s="70"/>
       <c r="B149" s="21"/>
       <c r="C149" s="48" t="s">
         <v>247</v>
@@ -10999,7 +11005,7 @@
       </c>
     </row>
     <row r="150" spans="1:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="A150" s="72"/>
+      <c r="A150" s="71"/>
       <c r="B150" s="21" t="s">
         <v>69</v>
       </c>
@@ -11041,7 +11047,7 @@
       </c>
     </row>
     <row r="151" spans="1:14" ht="390" x14ac:dyDescent="0.25">
-      <c r="A151" s="72"/>
+      <c r="A151" s="71"/>
       <c r="B151" s="21" t="s">
         <v>100</v>
       </c>
@@ -11128,7 +11134,7 @@
       </c>
     </row>
     <row r="152" spans="1:14" ht="150" x14ac:dyDescent="0.25">
-      <c r="A152" s="72"/>
+      <c r="A152" s="71"/>
       <c r="B152" s="21" t="s">
         <v>101</v>
       </c>
@@ -11170,7 +11176,7 @@
       </c>
     </row>
     <row r="153" spans="1:14" ht="75" x14ac:dyDescent="0.25">
-      <c r="A153" s="72"/>
+      <c r="A153" s="71"/>
       <c r="B153" s="21" t="s">
         <v>75</v>
       </c>
@@ -12422,7 +12428,7 @@
       <c r="N178" s="67"/>
     </row>
     <row r="179" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A179" s="71" t="s">
+      <c r="A179" s="68" t="s">
         <v>24</v>
       </c>
       <c r="B179" s="20" t="s">
@@ -12466,7 +12472,7 @@
       </c>
     </row>
     <row r="180" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A180" s="71"/>
+      <c r="A180" s="68"/>
       <c r="B180" s="21"/>
       <c r="C180" s="55" t="s">
         <v>112</v>
@@ -12722,7 +12728,7 @@
       <c r="O185" s="40"/>
     </row>
     <row r="186" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A186" s="71" t="s">
+      <c r="A186" s="68" t="s">
         <v>25</v>
       </c>
       <c r="B186" s="20" t="s">
@@ -12766,7 +12772,7 @@
       </c>
     </row>
     <row r="187" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A187" s="71"/>
+      <c r="A187" s="68"/>
       <c r="B187" s="21"/>
       <c r="C187" s="55" t="s">
         <v>112</v>
@@ -13016,7 +13022,7 @@
       </c>
     </row>
     <row r="193" spans="1:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="A193" s="71" t="s">
+      <c r="A193" s="68" t="s">
         <v>26</v>
       </c>
       <c r="B193" s="20" t="s">
@@ -13270,7 +13276,7 @@
       </c>
     </row>
     <row r="199" spans="1:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="A199" s="71" t="s">
+      <c r="A199" s="68" t="s">
         <v>27</v>
       </c>
       <c r="B199" s="20" t="s">
@@ -13314,7 +13320,7 @@
       </c>
     </row>
     <row r="200" spans="1:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="A200" s="71"/>
+      <c r="A200" s="68"/>
       <c r="B200" s="21" t="s">
         <v>69</v>
       </c>
@@ -13532,6 +13538,18 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A50:A53"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="A32:A35"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="A44:A48"/>
     <mergeCell ref="A199:A205"/>
     <mergeCell ref="A54:A57"/>
     <mergeCell ref="A59:A62"/>
@@ -13544,18 +13562,6 @@
     <mergeCell ref="A179:A184"/>
     <mergeCell ref="A186:A191"/>
     <mergeCell ref="A193:A197"/>
-    <mergeCell ref="A50:A53"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="A28:A31"/>
-    <mergeCell ref="A32:A35"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="A44:A48"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>